<commit_message>
u: added promotions and time management
</commit_message>
<xml_diff>
--- a/docs/timeleft.xlsx
+++ b/docs/timeleft.xlsx
@@ -104,8 +104,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,7 +424,7 @@
   <dimension ref="B2:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,15 +444,15 @@
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>45</v>
+      <c r="C3" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>30</v>
       </c>
     </row>
@@ -459,7 +460,7 @@
       <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>30</v>
       </c>
     </row>
@@ -467,15 +468,15 @@
       <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="C6">
-        <v>30</v>
+      <c r="C6" s="1">
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>5</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>90</v>
       </c>
     </row>
@@ -483,7 +484,7 @@
       <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>120</v>
       </c>
     </row>
@@ -491,7 +492,7 @@
       <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>120</v>
       </c>
     </row>
@@ -499,7 +500,7 @@
       <c r="B10" t="s">
         <v>8</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>45</v>
       </c>
     </row>
@@ -507,7 +508,7 @@
       <c r="B11" t="s">
         <v>9</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>120</v>
       </c>
     </row>
@@ -515,7 +516,7 @@
       <c r="B12" t="s">
         <v>11</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>45</v>
       </c>
     </row>
@@ -523,24 +524,30 @@
       <c r="B13" t="s">
         <v>12</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>120</v>
       </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C15" s="1"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>13</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <f>SUM(C3:C15)</f>
-        <v>795</v>
+        <v>740</v>
       </c>
       <c r="D16" t="s">
         <v>14</v>
       </c>
       <c r="E16">
         <f>C16/60</f>
-        <v>13.25</v>
+        <v>12.333333333333334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
u: added bug desc. & implemented counter graphics
</commit_message>
<xml_diff>
--- a/docs/timeleft.xlsx
+++ b/docs/timeleft.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\My Documents\Y2\Checkers Project\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Rahul\Documents\A levels\cs_checkers_a\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -200,6 +200,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -235,6 +252,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -390,7 +424,7 @@
   <dimension ref="B2:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,7 +453,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="1">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
@@ -427,7 +461,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="1">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
@@ -506,14 +540,14 @@
       </c>
       <c r="C16" s="1">
         <f>SUM(C3:C15)</f>
-        <v>710</v>
+        <v>650</v>
       </c>
       <c r="D16" t="s">
         <v>14</v>
       </c>
       <c r="E16">
         <f>C16/60</f>
-        <v>11.833333333333334</v>
+        <v>10.833333333333334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
u: added to timelift list
</commit_message>
<xml_diff>
--- a/docs/timeleft.xlsx
+++ b/docs/timeleft.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>task</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>in hrs --&gt;</t>
+  </si>
+  <si>
+    <t>win conditions</t>
   </si>
 </sst>
 </file>
@@ -421,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E16"/>
+  <dimension ref="B2:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,7 +435,7 @@
     <col min="2" max="2" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -440,7 +443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -448,7 +451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>10</v>
       </c>
@@ -456,98 +459,106 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C6" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C7" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>5</v>
-      </c>
-      <c r="C7" s="1">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>6</v>
       </c>
       <c r="C8" s="1">
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C10" s="1">
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C11" s="1">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C12" s="1">
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C13" s="1">
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C14" s="1">
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="1">
-        <f>SUM(C3:C15)</f>
-        <v>650</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="C17" s="1">
+        <f>SUM(C3:C16)</f>
+        <v>690</v>
+      </c>
+      <c r="D17" t="s">
         <v>14</v>
       </c>
-      <c r="E16">
-        <f>C16/60</f>
-        <v>10.833333333333334</v>
+      <c r="E17">
+        <f>C17/60</f>
+        <v>11.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
u: Analysis & MM tree
</commit_message>
<xml_diff>
--- a/docs/timeleft.xlsx
+++ b/docs/timeleft.xlsx
@@ -427,7 +427,7 @@
   <dimension ref="B2:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,7 +464,7 @@
         <v>15</v>
       </c>
       <c r="C5" s="1">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
@@ -480,7 +480,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="1">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
@@ -496,7 +496,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="1">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
@@ -512,7 +512,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="1">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
@@ -520,7 +520,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="1">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
@@ -551,14 +551,14 @@
       </c>
       <c r="C17" s="1">
         <f>SUM(C3:C16)</f>
-        <v>690</v>
+        <v>575</v>
       </c>
       <c r="D17" t="s">
         <v>14</v>
       </c>
       <c r="E17">
         <f>C17/60</f>
-        <v>11.5</v>
+        <v>9.5833333333333339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>